<commit_message>
SL ML Liveclass Practice and Demos
</commit_message>
<xml_diff>
--- a/regression.xlsx
+++ b/regression.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\Data Science\SL Python Books &amp; Labs\Course_3_LiveClassVideo_Machine_Learning\23 Sept Class Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,8 +24,138 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>dell</author>
+  </authors>
+  <commentList>
+    <comment ref="O4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+R-squared</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mean Absolute Error</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K9" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+RSS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Mean Squared Error</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dell:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Root Mean Squared Error</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Area</t>
   </si>
@@ -60,13 +191,70 @@
   </si>
   <si>
     <t>Sq Error</t>
+  </si>
+  <si>
+    <t>Absolute Error</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>Radio</t>
+  </si>
+  <si>
+    <t>Newspaper</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Degree 2</t>
+  </si>
+  <si>
+    <t>Degree 3</t>
+  </si>
+  <si>
+    <t>Degree 5</t>
+  </si>
+  <si>
+    <t>Degree 10</t>
+  </si>
+  <si>
+    <t>Degree 30</t>
+  </si>
+  <si>
+    <t>Simple Linear Regression</t>
+  </si>
+  <si>
+    <t>MLR</t>
+  </si>
+  <si>
+    <t>Polynomial Regression</t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t>R-squared</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +276,37 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="5">
@@ -169,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -178,11 +397,26 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,43 +696,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="12" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.28515625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C1" t="s">
+    <row r="1" spans="1:15">
+      <c r="C1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="45">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="10" t="s">
         <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -519,131 +757,144 @@
       <c r="I2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15">
       <c r="A3" s="7">
         <v>12</v>
       </c>
       <c r="B3" s="7">
         <v>45</v>
       </c>
-      <c r="C3" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C3" s="11">
+        <f t="shared" ref="C3:C8" si="0">AVERAGE($B$3:$B$8)</f>
         <v>74.5</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="9">
         <f>B3-C3</f>
         <v>-29.5</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <f>D3*D3</f>
         <v>870.25</v>
       </c>
       <c r="F3" s="4">
-        <f>$M$3</f>
+        <f>$N$3</f>
         <v>0.5</v>
       </c>
       <c r="G3" s="5">
-        <f>$M$4</f>
+        <f>$N$4</f>
         <v>1.9</v>
       </c>
       <c r="H3">
-        <f>G3*A3+F3</f>
-        <v>23.299999999999997</v>
+        <v>50</v>
       </c>
       <c r="I3">
         <f>B3-H3</f>
-        <v>21.700000000000003</v>
+        <v>-5</v>
       </c>
       <c r="J3">
+        <f>ABS(I3)</f>
+        <v>5</v>
+      </c>
+      <c r="K3">
         <f>I3*I3</f>
-        <v>470.8900000000001</v>
-      </c>
-      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
         <v>6</v>
       </c>
-      <c r="M3" s="4">
+      <c r="N3" s="4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15">
       <c r="A4" s="7">
         <v>35</v>
       </c>
       <c r="B4" s="7">
         <v>95</v>
       </c>
-      <c r="C4" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C4" s="11">
+        <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D4" s="10">
-        <f t="shared" ref="D4:D8" si="0">B4-C4</f>
+      <c r="D4" s="9">
+        <f t="shared" ref="D4:D8" si="1">B4-C4</f>
         <v>20.5</v>
       </c>
-      <c r="E4" s="10">
-        <f t="shared" ref="E4:E8" si="1">D4*D4</f>
+      <c r="E4" s="9">
+        <f t="shared" ref="E4:E8" si="2">D4*D4</f>
         <v>420.25</v>
       </c>
       <c r="F4" s="4">
-        <f t="shared" ref="F4:F8" si="2">$M$3</f>
+        <f t="shared" ref="F4:F8" si="3">$N$3</f>
         <v>0.5</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" ref="G4:G8" si="3">$M$4</f>
+        <f t="shared" ref="G4:G8" si="4">$N$4</f>
         <v>1.9</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H8" si="4">G4*A4+F4</f>
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="I4">
         <f t="shared" ref="I4:I8" si="5">B4-H4</f>
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J8" si="6">I4*I4</f>
-        <v>784</v>
-      </c>
-      <c r="L4" t="s">
+        <f t="shared" ref="J4:J8" si="6">ABS(I4)</f>
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4:K8" si="7">I4*I4</f>
+        <v>4</v>
+      </c>
+      <c r="M4" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="5">
+      <c r="N4" s="5">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <f>(E9-K9)/E9</f>
+        <v>0.35485826001955034</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="7">
         <v>24</v>
       </c>
       <c r="B5" s="7">
         <v>56</v>
       </c>
-      <c r="C5" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C5" s="11">
+        <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D5" s="10">
-        <f t="shared" si="0"/>
+      <c r="D5" s="9">
+        <f t="shared" si="1"/>
         <v>-18.5</v>
       </c>
-      <c r="E5" s="10">
-        <f t="shared" si="1"/>
+      <c r="E5" s="9">
+        <f t="shared" si="2"/>
         <v>342.25</v>
       </c>
       <c r="F5" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G5" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9</v>
       </c>
       <c r="H5">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H5:H7" si="8">G5*A5+F5</f>
         <v>46.099999999999994</v>
       </c>
       <c r="I5">
@@ -652,38 +903,42 @@
       </c>
       <c r="J5">
         <f t="shared" si="6"/>
+        <v>9.9000000000000057</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="7"/>
         <v>98.010000000000119</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15">
       <c r="A6" s="7">
         <v>10</v>
       </c>
       <c r="B6" s="7">
         <v>32</v>
       </c>
-      <c r="C6" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C6" s="11">
+        <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D6" s="10">
-        <f t="shared" si="0"/>
+      <c r="D6" s="9">
+        <f t="shared" si="1"/>
         <v>-42.5</v>
       </c>
-      <c r="E6" s="10">
-        <f t="shared" si="1"/>
+      <c r="E6" s="9">
+        <f t="shared" si="2"/>
         <v>1806.25</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G6" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9</v>
       </c>
       <c r="H6">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19.5</v>
       </c>
       <c r="I6">
@@ -692,38 +947,42 @@
       </c>
       <c r="J6">
         <f t="shared" si="6"/>
+        <v>12.5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="7"/>
         <v>156.25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15">
       <c r="A7" s="7">
         <v>56</v>
       </c>
       <c r="B7" s="7">
         <v>90</v>
       </c>
-      <c r="C7" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C7" s="11">
+        <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D7" s="10">
-        <f t="shared" si="0"/>
+      <c r="D7" s="9">
+        <f t="shared" si="1"/>
         <v>15.5</v>
       </c>
-      <c r="E7" s="10">
-        <f t="shared" si="1"/>
+      <c r="E7" s="9">
+        <f t="shared" si="2"/>
         <v>240.25</v>
       </c>
       <c r="F7" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G7" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9</v>
       </c>
       <c r="H7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>106.89999999999999</v>
       </c>
       <c r="I7">
@@ -732,70 +991,311 @@
       </c>
       <c r="J7">
         <f t="shared" si="6"/>
+        <v>16.899999999999991</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="7"/>
         <v>285.60999999999973</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="7">
         <v>104</v>
       </c>
       <c r="B8" s="7">
         <v>129</v>
       </c>
-      <c r="C8" s="10">
-        <f>AVERAGE($B$3:$B$8)</f>
+      <c r="C8" s="11">
+        <f t="shared" si="0"/>
         <v>74.5</v>
       </c>
-      <c r="D8" s="10">
-        <f t="shared" si="0"/>
+      <c r="D8" s="9">
+        <f t="shared" si="1"/>
         <v>54.5</v>
       </c>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
+      <c r="E8" s="9">
+        <f t="shared" si="2"/>
         <v>2970.25</v>
       </c>
       <c r="F8" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.9</v>
       </c>
       <c r="H8">
-        <f t="shared" si="4"/>
-        <v>198.1</v>
+        <v>190</v>
       </c>
       <c r="I8">
         <f t="shared" si="5"/>
-        <v>-69.099999999999994</v>
+        <v>-61</v>
       </c>
       <c r="J8">
         <f t="shared" si="6"/>
-        <v>4774.8099999999995</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D9" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="7"/>
+        <v>3721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="D9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <f>SUM(E3:E8)</f>
         <v>6649.5</v>
       </c>
-      <c r="I9" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J9" s="3">
-        <f>SUM(J3:J8)</f>
-        <v>6569.57</v>
+      <c r="J9" s="2">
+        <f>AVERAGE(J3:J8)</f>
+        <v>17.883333333333333</v>
+      </c>
+      <c r="K9" s="3">
+        <f>SUM(K3:K8)</f>
+        <v>4289.87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="K10" s="8">
+        <f>AVERAGE(K3:K8)</f>
+        <v>714.97833333333335</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="K11" s="8">
+        <f>SQRT(K10)</f>
+        <v>26.73907876747689</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:J1"/>
+  <mergeCells count="2">
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="C1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2.55971718495804</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="7">
+        <v>10.892105452487399</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3.3003189925350198</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.62324347610284603</v>
+      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="4:4">
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="4:4">
+      <c r="D18" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="G3:K3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>